<commit_message>
updated model run with climate change scenario
</commit_message>
<xml_diff>
--- a/processed_data/Capacity_factors/Reference/REF_WeeklyFlow.xlsx
+++ b/processed_data/Capacity_factors/Reference/REF_WeeklyFlow.xlsx
@@ -438,28 +438,28 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>25.31226969696968</v>
+        <v>26.83665211640207</v>
       </c>
       <c r="C2">
-        <v>4.941728601252606</v>
+        <v>7.070460035523974</v>
       </c>
       <c r="D2">
-        <v>21.15679469696972</v>
+        <v>31.90594246031748</v>
       </c>
       <c r="E2">
-        <v>32.15745833333331</v>
+        <v>50.89867923280419</v>
       </c>
       <c r="F2">
-        <v>84.67006818181812</v>
+        <v>112.3310965608466</v>
       </c>
       <c r="G2">
-        <v>91.35120619396901</v>
+        <v>101.2979774489077</v>
       </c>
       <c r="H2">
-        <v>82.49064786585359</v>
+        <v>115.9774268617022</v>
       </c>
       <c r="I2">
-        <v>20.63526315789476</v>
+        <v>25.14072727272729</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -467,28 +467,28 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>30.82524032738094</v>
+        <v>31.20065211640209</v>
       </c>
       <c r="C3">
-        <v>7.18244537114261</v>
+        <v>7.403211411850752</v>
       </c>
       <c r="D3">
-        <v>29.64313541666666</v>
+        <v>32.71234722222221</v>
       </c>
       <c r="E3">
-        <v>40.32766369047628</v>
+        <v>51.81736441798948</v>
       </c>
       <c r="F3">
-        <v>103.9765885416668</v>
+        <v>124.4400601851853</v>
       </c>
       <c r="G3">
-        <v>83.36165095986047</v>
+        <v>114.1155745814308</v>
       </c>
       <c r="H3">
-        <v>111.0703122619955</v>
+        <v>146.1445104659014</v>
       </c>
       <c r="I3">
-        <v>21.78317919075143</v>
+        <v>30.30559701492537</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -496,28 +496,28 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>28.77114285714278</v>
+        <v>31.66342592592583</v>
       </c>
       <c r="C4">
-        <v>5.132065176908754</v>
+        <v>4.937098650927489</v>
       </c>
       <c r="D4">
-        <v>16.77345190839694</v>
+        <v>17.34552368064952</v>
       </c>
       <c r="E4">
-        <v>29.39712425595237</v>
+        <v>31.67509854497353</v>
       </c>
       <c r="F4">
-        <v>82.83433630952365</v>
+        <v>83.45353174603166</v>
       </c>
       <c r="G4">
-        <v>102.0480454183268</v>
+        <v>109.9871890372454</v>
       </c>
       <c r="H4">
-        <v>117.8924553571428</v>
+        <v>124.06041005291</v>
       </c>
       <c r="I4">
-        <v>28.0084244897959</v>
+        <v>34.24274946159363</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -525,28 +525,28 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>30.53484523809521</v>
+        <v>34.38846097883595</v>
       </c>
       <c r="C5">
-        <v>5.411126984126984</v>
+        <v>5.158487200000001</v>
       </c>
       <c r="D5">
-        <v>18.1406171243942</v>
+        <v>17.81064722617356</v>
       </c>
       <c r="E5">
-        <v>38.47142559523807</v>
+        <v>37.45637433862433</v>
       </c>
       <c r="F5">
-        <v>96.3464754464285</v>
+        <v>92.30152182539668</v>
       </c>
       <c r="G5">
-        <v>65.36442027455116</v>
+        <v>74.02027713004478</v>
       </c>
       <c r="H5">
-        <v>123.3327529761906</v>
+        <v>117.5038161375662</v>
       </c>
       <c r="I5">
-        <v>34.43684756584197</v>
+        <v>33.55907811400419</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -554,28 +554,28 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>28.16706175595241</v>
+        <v>33.22866732804237</v>
       </c>
       <c r="C6">
-        <v>6.784197492163017</v>
+        <v>7.209011772853199</v>
       </c>
       <c r="D6">
-        <v>19.8510904480135</v>
+        <v>20.11536343449294</v>
       </c>
       <c r="E6">
-        <v>39.18654241071425</v>
+        <v>38.63712367724865</v>
       </c>
       <c r="F6">
-        <v>88.40506398809534</v>
+        <v>90.47859920634927</v>
       </c>
       <c r="G6">
-        <v>73.39224918032788</v>
+        <v>69.86248244958929</v>
       </c>
       <c r="H6">
-        <v>73.86269492808485</v>
+        <v>79.30388179986572</v>
       </c>
       <c r="I6">
-        <v>23.77528169014083</v>
+        <v>24.33154999999998</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -583,28 +583,28 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>25.49720386904759</v>
+        <v>31.23341600529097</v>
       </c>
       <c r="C7">
-        <v>6.01368861347792</v>
+        <v>6.596995844875346</v>
       </c>
       <c r="D7">
-        <v>17.74465550595239</v>
+        <v>18.11013690476191</v>
       </c>
       <c r="E7">
-        <v>33.74597321428574</v>
+        <v>34.08775330687831</v>
       </c>
       <c r="F7">
-        <v>79.54641517857155</v>
+        <v>88.86810582010584</v>
       </c>
       <c r="G7">
-        <v>67.34341889880939</v>
+        <v>64.84887842586076</v>
       </c>
       <c r="H7">
-        <v>101.7454389880951</v>
+        <v>124.9394775132273</v>
       </c>
       <c r="I7">
-        <v>21.69422945205479</v>
+        <v>22.83711493354182</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -612,28 +612,28 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>24.31511681547621</v>
+        <v>29.42128174603172</v>
       </c>
       <c r="C8">
-        <v>5.565888012618297</v>
+        <v>6.781230501392759</v>
       </c>
       <c r="D8">
-        <v>20.86072790161417</v>
+        <v>26.06118039482642</v>
       </c>
       <c r="E8">
-        <v>32.44699776785716</v>
+        <v>44.24564682539686</v>
       </c>
       <c r="F8">
-        <v>92.89975892857147</v>
+        <v>109.9479047619048</v>
       </c>
       <c r="G8">
-        <v>73.74150139794976</v>
+        <v>72.30011121076242</v>
       </c>
       <c r="H8">
-        <v>112.3715029761905</v>
+        <v>124.0523412698413</v>
       </c>
       <c r="I8">
-        <v>29.63407944996186</v>
+        <v>31.44227982954548</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -641,28 +641,28 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>23.11820163690478</v>
+        <v>27.71380158730158</v>
       </c>
       <c r="C9">
-        <v>4.571008496176725</v>
+        <v>6.541176951672868</v>
       </c>
       <c r="D9">
-        <v>24.12500446428572</v>
+        <v>34.004</v>
       </c>
       <c r="E9">
-        <v>38.57128050595242</v>
+        <v>60.49908664021164</v>
       </c>
       <c r="F9">
-        <v>110.7807477678573</v>
+        <v>139.09285978836</v>
       </c>
       <c r="G9">
-        <v>103.886920207254</v>
+        <v>119.6991067961166</v>
       </c>
       <c r="H9">
-        <v>85.58423135464234</v>
+        <v>112.6196693657221</v>
       </c>
       <c r="I9">
-        <v>28.43647717484924</v>
+        <v>34.10984150943393</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -670,28 +670,28 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>25.86942931547619</v>
+        <v>29.75482076719578</v>
       </c>
       <c r="C10">
-        <v>6.367279202279208</v>
+        <v>7.125958230958235</v>
       </c>
       <c r="D10">
-        <v>26.34910491071427</v>
+        <v>32.89399669312166</v>
       </c>
       <c r="E10">
-        <v>49.7185007440476</v>
+        <v>64.95560582010575</v>
       </c>
       <c r="F10">
-        <v>107.6029732142857</v>
+        <v>120.2013134920635</v>
       </c>
       <c r="G10">
-        <v>104.9452585616439</v>
+        <v>122.4533824850301</v>
       </c>
       <c r="H10">
-        <v>137.1436976744189</v>
+        <v>156.5086282578877</v>
       </c>
       <c r="I10">
-        <v>28.16761403508775</v>
+        <v>37.54267584097862</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -699,28 +699,28 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>26.93365773809521</v>
+        <v>31.70006481481479</v>
       </c>
       <c r="C11">
-        <v>6.271283151326049</v>
+        <v>6.936157931034484</v>
       </c>
       <c r="D11">
-        <v>30.17615476190476</v>
+        <v>30.55407539682541</v>
       </c>
       <c r="E11">
-        <v>62.90319866071443</v>
+        <v>66.68659457671973</v>
       </c>
       <c r="F11">
-        <v>147.0923065476192</v>
+        <v>150.3394563492065</v>
       </c>
       <c r="G11">
-        <v>117.456685820204</v>
+        <v>124.0807602245389</v>
       </c>
       <c r="H11">
-        <v>123.5986159695818</v>
+        <v>141.9624072825356</v>
       </c>
       <c r="I11">
-        <v>25.18587096774194</v>
+        <v>30.39456284153005</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -728,28 +728,28 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>26.73074330357138</v>
+        <v>31.13147949735443</v>
       </c>
       <c r="C12">
-        <v>5.324664037854897</v>
+        <v>5.546353760445689</v>
       </c>
       <c r="D12">
-        <v>28.37523586309525</v>
+        <v>28.17324933862432</v>
       </c>
       <c r="E12">
-        <v>45.84598214285716</v>
+        <v>47.55922883597884</v>
       </c>
       <c r="F12">
-        <v>114.1586770833332</v>
+        <v>112.8410496031745</v>
       </c>
       <c r="G12">
-        <v>93.23923951048954</v>
+        <v>99.70266539634152</v>
       </c>
       <c r="H12">
-        <v>131.6197767857142</v>
+        <v>131.5535449735449</v>
       </c>
       <c r="I12">
-        <v>33.65435285053927</v>
+        <v>35.54130286493859</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -757,28 +757,28 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>25.59073735119047</v>
+        <v>30.55336574074073</v>
       </c>
       <c r="C13">
-        <v>3.889523684210523</v>
+        <v>3.877964506172834</v>
       </c>
       <c r="D13">
-        <v>33.52540848214284</v>
+        <v>37.01627116402116</v>
       </c>
       <c r="E13">
-        <v>54.56026339285708</v>
+        <v>57.49600529100528</v>
       </c>
       <c r="F13">
-        <v>91.16330208333333</v>
+        <v>89.28547156084656</v>
       </c>
       <c r="G13">
-        <v>80.54772588832476</v>
+        <v>77.44795844625104</v>
       </c>
       <c r="H13">
-        <v>115.6294270833336</v>
+        <v>110.83210978836</v>
       </c>
       <c r="I13">
-        <v>33.52868552412648</v>
+        <v>32.23346715328472</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -786,28 +786,28 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>26.0414613095238</v>
+        <v>30.52379298941796</v>
       </c>
       <c r="C14">
-        <v>5.683699702675917</v>
+        <v>5.420098555649957</v>
       </c>
       <c r="D14">
-        <v>46.06270907738095</v>
+        <v>47.4778035714286</v>
       </c>
       <c r="E14">
-        <v>73.23026636904758</v>
+        <v>75.49366005291009</v>
       </c>
       <c r="F14">
-        <v>119.1120825892859</v>
+        <v>114.1752056878309</v>
       </c>
       <c r="G14">
-        <v>75.28992890995264</v>
+        <v>72.12960343417825</v>
       </c>
       <c r="H14">
-        <v>91.48333841463422</v>
+        <v>87.58845270270275</v>
       </c>
       <c r="I14">
-        <v>24.26776954732512</v>
+        <v>24.10151120751989</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -815,28 +815,28 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>27.83821056547614</v>
+        <v>31.12391137566135</v>
       </c>
       <c r="C15">
-        <v>5.124752860411906</v>
+        <v>4.723283109404997</v>
       </c>
       <c r="D15">
-        <v>39.80018526785721</v>
+        <v>40.19235912698418</v>
       </c>
       <c r="E15">
-        <v>54.27682440476192</v>
+        <v>58.7381309523809</v>
       </c>
       <c r="F15">
-        <v>76.40182738095253</v>
+        <v>74.36631679894191</v>
       </c>
       <c r="G15">
-        <v>118.2447317282891</v>
+        <v>114.7039609316304</v>
       </c>
       <c r="H15">
-        <v>106.3999330357143</v>
+        <v>102.0950396825396</v>
       </c>
       <c r="I15">
-        <v>26.67835983263601</v>
+        <v>25.47469552457813</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -844,28 +844,28 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>29.82559151785723</v>
+        <v>33.05881415343924</v>
       </c>
       <c r="C16">
-        <v>3.329397101449278</v>
+        <v>3.294448046550294</v>
       </c>
       <c r="D16">
-        <v>42.4478407738095</v>
+        <v>46.01707142857141</v>
       </c>
       <c r="E16">
-        <v>62.39840848214286</v>
+        <v>71.25693320105812</v>
       </c>
       <c r="F16">
-        <v>79.31052455357137</v>
+        <v>84.20055489417977</v>
       </c>
       <c r="G16">
-        <v>69.93540210526318</v>
+        <v>70.03778100775196</v>
       </c>
       <c r="H16">
-        <v>136.7976190476188</v>
+        <v>136.0149663526242</v>
       </c>
       <c r="I16">
-        <v>23.18696369636964</v>
+        <v>24.21552460538533</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -873,28 +873,28 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>32.71298139880952</v>
+        <v>36.4650357142857</v>
       </c>
       <c r="C17">
-        <v>3.993258132214063</v>
+        <v>4.197031934306573</v>
       </c>
       <c r="D17">
-        <v>33.11267633928572</v>
+        <v>39.30351124338623</v>
       </c>
       <c r="E17">
-        <v>55.11718526785715</v>
+        <v>66.62775000000001</v>
       </c>
       <c r="F17">
-        <v>77.62708184523834</v>
+        <v>87.94780621693141</v>
       </c>
       <c r="G17">
-        <v>73.96612941176475</v>
+        <v>90.15460690235697</v>
       </c>
       <c r="H17">
-        <v>129.0970014880954</v>
+        <v>135.2234946949602</v>
       </c>
       <c r="I17">
-        <v>31.89815158546018</v>
+        <v>32.62356990773598</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -902,28 +902,28 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>31.42672842261911</v>
+        <v>34.87846759259265</v>
       </c>
       <c r="C18">
-        <v>4.617546122448983</v>
+        <v>4.566334529791817</v>
       </c>
       <c r="D18">
-        <v>32.36776264880958</v>
+        <v>34.28830224867729</v>
       </c>
       <c r="E18">
-        <v>44.80755877976191</v>
+        <v>49.57275859788358</v>
       </c>
       <c r="F18">
-        <v>60.31227678571428</v>
+        <v>62.08713558201061</v>
       </c>
       <c r="G18">
-        <v>71.71495023474176</v>
+        <v>79.24955474452555</v>
       </c>
       <c r="H18">
-        <v>92.13192708333328</v>
+        <v>99.05015873015866</v>
       </c>
       <c r="I18">
-        <v>20.17271132376393</v>
+        <v>25.06654711673696</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -931,28 +931,28 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>32.40188244047617</v>
+        <v>35.02670701058195</v>
       </c>
       <c r="C19">
-        <v>3.695532727272729</v>
+        <v>3.530049684542593</v>
       </c>
       <c r="D19">
-        <v>32.41238392857142</v>
+        <v>32.76374272486772</v>
       </c>
       <c r="E19">
-        <v>37.77454538690474</v>
+        <v>40.63878240740741</v>
       </c>
       <c r="F19">
-        <v>54.12241443452382</v>
+        <v>54.25959523809528</v>
       </c>
       <c r="G19">
-        <v>63.75369528301884</v>
+        <v>70.65936563517907</v>
       </c>
       <c r="H19">
-        <v>83.45731398809519</v>
+        <v>83.73421296296291</v>
       </c>
       <c r="I19">
-        <v>16.40611201298698</v>
+        <v>17.25985714285711</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -960,28 +960,28 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>30.18613616071429</v>
+        <v>33.17596494708996</v>
       </c>
       <c r="C20">
-        <v>4.483722162162159</v>
+        <v>4.186491329479764</v>
       </c>
       <c r="D20">
-        <v>31.22649255952388</v>
+        <v>31.1878108465609</v>
       </c>
       <c r="E20">
-        <v>39.07519642857143</v>
+        <v>41.23272751322752</v>
       </c>
       <c r="F20">
-        <v>55.62913318452379</v>
+        <v>55.66090939153438</v>
       </c>
       <c r="G20">
-        <v>55.32565160642568</v>
+        <v>59.19846012269936</v>
       </c>
       <c r="H20">
-        <v>95.19759672619062</v>
+        <v>100.9448082010584</v>
       </c>
       <c r="I20">
-        <v>14.48181338028168</v>
+        <v>19.61801380368098</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -989,28 +989,28 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>27.67689360119043</v>
+        <v>31.02996362433858</v>
       </c>
       <c r="C21">
-        <v>3.691199265381086</v>
+        <v>4.089845664280034</v>
       </c>
       <c r="D21">
-        <v>28.1285357142857</v>
+        <v>30.08063492063491</v>
       </c>
       <c r="E21">
-        <v>33.35155952380954</v>
+        <v>36.86551719576718</v>
       </c>
       <c r="F21">
-        <v>56.34225000000007</v>
+        <v>58.75122817460321</v>
       </c>
       <c r="G21">
-        <v>58.29546090156401</v>
+        <v>59.44855686604899</v>
       </c>
       <c r="H21">
-        <v>85.08988095238081</v>
+        <v>92.04526455026438</v>
       </c>
       <c r="I21">
-        <v>15.99028309104819</v>
+        <v>19.8282033898305</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1018,28 +1018,28 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>26.14113244047615</v>
+        <v>29.22908002645496</v>
       </c>
       <c r="C22">
-        <v>3.743749736008447</v>
+        <v>3.511602888086645</v>
       </c>
       <c r="D22">
-        <v>24.07142559523808</v>
+        <v>24.12733730158729</v>
       </c>
       <c r="E22">
-        <v>25.35578497023809</v>
+        <v>27.04519113756607</v>
       </c>
       <c r="F22">
-        <v>41.63065327380948</v>
+        <v>41.98066335978829</v>
       </c>
       <c r="G22">
-        <v>61.32114625850343</v>
+        <v>66.34005654761907</v>
       </c>
       <c r="H22">
-        <v>72.09263392857142</v>
+        <v>72.80135582010583</v>
       </c>
       <c r="I22">
-        <v>12.68681739130434</v>
+        <v>13.40291350531106</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1047,28 +1047,28 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>26.98997098214283</v>
+        <v>30.17985052910049</v>
       </c>
       <c r="C23">
-        <v>2.258218400687873</v>
+        <v>2.165046581517653</v>
       </c>
       <c r="D23">
-        <v>21.44070907738097</v>
+        <v>21.21713624338627</v>
       </c>
       <c r="E23">
-        <v>23.59396949404761</v>
+        <v>24.44210912698413</v>
       </c>
       <c r="F23">
-        <v>37.88268675595242</v>
+        <v>38.09431547619054</v>
       </c>
       <c r="G23">
-        <v>50.53617398945515</v>
+        <v>53.91978483920359</v>
       </c>
       <c r="H23">
-        <v>74.51277529761893</v>
+        <v>76.340443121693</v>
       </c>
       <c r="I23">
-        <v>12.74633709981168</v>
+        <v>13.63191769547326</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1076,28 +1076,28 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>27.91332366071429</v>
+        <v>31.06386243386246</v>
       </c>
       <c r="C24">
-        <v>2.840224101479916</v>
+        <v>2.628951526032316</v>
       </c>
       <c r="D24">
-        <v>22.35292336309523</v>
+        <v>21.42189484126983</v>
       </c>
       <c r="E24">
-        <v>25.5710178571429</v>
+        <v>25.17070436507941</v>
       </c>
       <c r="F24">
-        <v>43.12771949404765</v>
+        <v>41.92285052910052</v>
       </c>
       <c r="G24">
-        <v>31.67735089463222</v>
+        <v>36.54026746166953</v>
       </c>
       <c r="H24">
-        <v>107.2720014880953</v>
+        <v>101.6619378306879</v>
       </c>
       <c r="I24">
-        <v>16.41482039397448</v>
+        <v>16.22907856450044</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1105,28 +1105,28 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>21.48020610119048</v>
+        <v>25.32777910052911</v>
       </c>
       <c r="C25">
-        <v>5.310435483870966</v>
+        <v>4.796918276374441</v>
       </c>
       <c r="D25">
-        <v>22.29070312499998</v>
+        <v>20.93608994708993</v>
       </c>
       <c r="E25">
-        <v>19.86430729166666</v>
+        <v>19.96198544973543</v>
       </c>
       <c r="F25">
-        <v>35.87509002976194</v>
+        <v>35.15650264550264</v>
       </c>
       <c r="G25">
-        <v>38.47527380952378</v>
+        <v>39.58647395833335</v>
       </c>
       <c r="H25">
-        <v>79.86557291666662</v>
+        <v>76.68099867724864</v>
       </c>
       <c r="I25">
-        <v>19.64327828241124</v>
+        <v>18.50716265499636</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1134,28 +1134,28 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>22.08968898809524</v>
+        <v>25.8915687830688</v>
       </c>
       <c r="C26">
-        <v>3.471889848812097</v>
+        <v>3.18883180987203</v>
       </c>
       <c r="D26">
-        <v>19.47111160714285</v>
+        <v>18.94427447089946</v>
       </c>
       <c r="E26">
-        <v>15.38537202380952</v>
+        <v>15.70032936507937</v>
       </c>
       <c r="F26">
-        <v>27.99282440476184</v>
+        <v>28.33901322751318</v>
       </c>
       <c r="G26">
-        <v>41.99774424342107</v>
+        <v>40.50848699421969</v>
       </c>
       <c r="H26">
-        <v>57.35587053571426</v>
+        <v>57.06417989417987</v>
       </c>
       <c r="I26">
-        <v>10.8586038687973</v>
+        <v>11.56542372881355</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1163,28 +1163,28 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>28.07848735119053</v>
+        <v>30.54775992063499</v>
       </c>
       <c r="C27">
-        <v>1.302645833333334</v>
+        <v>1.558011363636364</v>
       </c>
       <c r="D27">
-        <v>15.86991653905053</v>
+        <v>15.69497354138396</v>
       </c>
       <c r="E27">
-        <v>12.76114657738094</v>
+        <v>12.89673082010581</v>
       </c>
       <c r="F27">
-        <v>26.66161086309525</v>
+        <v>26.65554298941803</v>
       </c>
       <c r="G27">
-        <v>32.21672575516695</v>
+        <v>32.42231346423561</v>
       </c>
       <c r="H27">
-        <v>55.7431770833334</v>
+        <v>53.76192460317473</v>
       </c>
       <c r="I27">
-        <v>10.38414796342477</v>
+        <v>10.2126311844078</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1192,28 +1192,28 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>27.13787574404755</v>
+        <v>28.96451917989414</v>
       </c>
       <c r="C28">
-        <v>1.313611831442462</v>
+        <v>1.362005706134091</v>
       </c>
       <c r="D28">
-        <v>15.77525170068028</v>
+        <v>15.27143824404762</v>
       </c>
       <c r="E28">
-        <v>10.22798511904763</v>
+        <v>10.39658333333333</v>
       </c>
       <c r="F28">
-        <v>24.11193452380951</v>
+        <v>24.00483333333333</v>
       </c>
       <c r="G28">
-        <v>25.99059226190476</v>
+        <v>27.26633994708997</v>
       </c>
       <c r="H28">
-        <v>40.56441220238092</v>
+        <v>38.95066137566135</v>
       </c>
       <c r="I28">
-        <v>10.84468005952381</v>
+        <v>10.72909391534391</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1221,28 +1221,28 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>23.27591889880958</v>
+        <v>24.31082936507942</v>
       </c>
       <c r="C29">
-        <v>1.986140613313388</v>
+        <v>2.162019933554818</v>
       </c>
       <c r="D29">
-        <v>15.4328734082397</v>
+        <v>15.26719361277446</v>
       </c>
       <c r="E29">
-        <v>8.962380208333343</v>
+        <v>9.052226190476198</v>
       </c>
       <c r="F29">
-        <v>20.66509375000001</v>
+        <v>20.69406150793652</v>
       </c>
       <c r="G29">
-        <v>24.19825818452382</v>
+        <v>25.31941269841271</v>
       </c>
       <c r="H29">
-        <v>30.40418154761902</v>
+        <v>29.84757275132272</v>
       </c>
       <c r="I29">
-        <v>6.932073170731708</v>
+        <v>6.809364620938626</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1250,28 +1250,28 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>24.05207886904764</v>
+        <v>23.37902976190478</v>
       </c>
       <c r="C30">
-        <v>2.074134680134681</v>
+        <v>3.29486402266289</v>
       </c>
       <c r="D30">
-        <v>14.51248065476191</v>
+        <v>14.68932076719577</v>
       </c>
       <c r="E30">
-        <v>8.072357886904758</v>
+        <v>8.133062169312167</v>
       </c>
       <c r="F30">
-        <v>19.17784598214287</v>
+        <v>19.30113425925927</v>
       </c>
       <c r="G30">
-        <v>22.79534226190478</v>
+        <v>23.61277380952384</v>
       </c>
       <c r="H30">
-        <v>27.21709821428573</v>
+        <v>27.21534391534392</v>
       </c>
       <c r="I30">
-        <v>7.157127831715212</v>
+        <v>7.178165938864637</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1279,28 +1279,28 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>24.49444791666664</v>
+        <v>25.2925304232804</v>
       </c>
       <c r="C31">
-        <v>1.254275830258304</v>
+        <v>1.252271062271064</v>
       </c>
       <c r="D31">
-        <v>12.28525818452381</v>
+        <v>12.69565145502645</v>
       </c>
       <c r="E31">
-        <v>8.747238095238075</v>
+        <v>8.622050264550245</v>
       </c>
       <c r="F31">
-        <v>17.86488839285713</v>
+        <v>17.93033465608464</v>
       </c>
       <c r="G31">
-        <v>22.55923488773749</v>
+        <v>22.87773453996983</v>
       </c>
       <c r="H31">
-        <v>23.07926339285713</v>
+        <v>23.73594576719576</v>
       </c>
       <c r="I31">
-        <v>4.650771678599829</v>
+        <v>5.249644670050748</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1308,28 +1308,28 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>22.98880133928573</v>
+        <v>24.08470634920637</v>
       </c>
       <c r="C32">
         <v>2.105780444444445</v>
       </c>
       <c r="D32">
-        <v>12.15025297619047</v>
+        <v>11.74354695767194</v>
       </c>
       <c r="E32">
-        <v>8.490686011904756</v>
+        <v>8.314541666666669</v>
       </c>
       <c r="F32">
-        <v>19.53196726190476</v>
+        <v>19.25848082010581</v>
       </c>
       <c r="G32">
-        <v>18.59509196428572</v>
+        <v>18.77296583850933</v>
       </c>
       <c r="H32">
-        <v>30.42102678571427</v>
+        <v>28.96178571428568</v>
       </c>
       <c r="I32">
-        <v>6.034093457943928</v>
+        <v>6.024046849757678</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1337,28 +1337,28 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>21.17453422619048</v>
+        <v>22.8080972222222</v>
       </c>
       <c r="C33">
-        <v>2.186056547619051</v>
+        <v>2.123181731684114</v>
       </c>
       <c r="D33">
-        <v>13.39327604166667</v>
+        <v>12.42561507936508</v>
       </c>
       <c r="E33">
-        <v>8.454860863095238</v>
+        <v>8.204949074074069</v>
       </c>
       <c r="F33">
-        <v>20.0314888392857</v>
+        <v>19.7069537037037</v>
       </c>
       <c r="G33">
-        <v>19.2861876675603</v>
+        <v>18.6555936285936</v>
       </c>
       <c r="H33">
-        <v>35.64900297619048</v>
+        <v>35.97556878306878</v>
       </c>
       <c r="I33">
-        <v>10.1705320945946</v>
+        <v>9.955450885668283</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1366,28 +1366,28 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>18.78991369047621</v>
+        <v>20.25136640211642</v>
       </c>
       <c r="C34">
-        <v>2.769842446709913</v>
+        <v>2.694327185244581</v>
       </c>
       <c r="D34">
-        <v>13.27215327380953</v>
+        <v>12.33151190476191</v>
       </c>
       <c r="E34">
-        <v>7.318575148809528</v>
+        <v>7.139550264550266</v>
       </c>
       <c r="F34">
-        <v>21.5295349702381</v>
+        <v>20.88180357142857</v>
       </c>
       <c r="G34">
-        <v>20.0523810741688</v>
+        <v>19.01493363161817</v>
       </c>
       <c r="H34">
-        <v>38.27877976190474</v>
+        <v>36.72531084656082</v>
       </c>
       <c r="I34">
-        <v>11.31892452830188</v>
+        <v>11.49447882736156</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1395,28 +1395,28 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>21.78750297619048</v>
+        <v>23.01520436507936</v>
       </c>
       <c r="C35">
-        <v>1.68221684414327</v>
+        <v>1.612757220216605</v>
       </c>
       <c r="D35">
-        <v>13.02285725552052</v>
+        <v>12.15616504178275</v>
       </c>
       <c r="E35">
-        <v>6.730769345238106</v>
+        <v>6.584408068783082</v>
       </c>
       <c r="F35">
-        <v>17.10918526785716</v>
+        <v>16.84762764550266</v>
       </c>
       <c r="G35">
-        <v>20.19499828473416</v>
+        <v>18.85211019490255</v>
       </c>
       <c r="H35">
-        <v>26.62757440476193</v>
+        <v>25.29438492063493</v>
       </c>
       <c r="I35">
-        <v>7.949504065040656</v>
+        <v>7.527603719599434</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1424,28 +1424,28 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>17.18850223214288</v>
+        <v>18.79240343915342</v>
       </c>
       <c r="C36">
-        <v>3.484859337105895</v>
+        <v>3.224835014409216</v>
       </c>
       <c r="D36">
-        <v>12.16485543964232</v>
+        <v>11.40357019867548</v>
       </c>
       <c r="E36">
-        <v>8.852898809523799</v>
+        <v>8.775236772486769</v>
       </c>
       <c r="F36">
-        <v>16.76423214285714</v>
+        <v>16.75009126984128</v>
       </c>
       <c r="G36">
-        <v>18.26168671679196</v>
+        <v>17.19679923954371</v>
       </c>
       <c r="H36">
-        <v>21.72405505952381</v>
+        <v>21.63763888888889</v>
       </c>
       <c r="I36">
-        <v>5.875256087321571</v>
+        <v>6.064888547271321</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1453,28 +1453,28 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>15.86316815476192</v>
+        <v>17.5944351851852</v>
       </c>
       <c r="C37">
-        <v>2.139302843966183</v>
+        <v>2.032147038801909</v>
       </c>
       <c r="D37">
-        <v>13.71671651785715</v>
+        <v>12.76958333333334</v>
       </c>
       <c r="E37">
-        <v>8.137998511904758</v>
+        <v>8.162468915343915</v>
       </c>
       <c r="F37">
-        <v>16.17650148809527</v>
+        <v>16.24723148148151</v>
       </c>
       <c r="G37">
-        <v>17.61640932642487</v>
+        <v>15.93598868778279</v>
       </c>
       <c r="H37">
-        <v>20.9061532738095</v>
+        <v>22.89031084656082</v>
       </c>
       <c r="I37">
-        <v>5.953361847733111</v>
+        <v>6.050719424460436</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1482,28 +1482,28 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>14.57790104166662</v>
+        <v>16.34774801587298</v>
       </c>
       <c r="C38">
-        <v>2.164262886597941</v>
+        <v>2.07438888888889</v>
       </c>
       <c r="D38">
-        <v>14.43467336309521</v>
+        <v>13.48683134920632</v>
       </c>
       <c r="E38">
-        <v>9.00175520833333</v>
+        <v>8.950611111111114</v>
       </c>
       <c r="F38">
-        <v>16.61539136904763</v>
+        <v>16.67379431216931</v>
       </c>
       <c r="G38">
-        <v>15.35405610859727</v>
+        <v>14.37217642405061</v>
       </c>
       <c r="H38">
-        <v>27.7537797619048</v>
+        <v>32.62683862433863</v>
       </c>
       <c r="I38">
-        <v>8.034660107334513</v>
+        <v>9.600604351329565</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1511,28 +1511,28 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>14.30061681547621</v>
+        <v>16.14714880952383</v>
       </c>
       <c r="C39">
-        <v>1.548191919191919</v>
+        <v>1.471407963936889</v>
       </c>
       <c r="D39">
-        <v>14.38352678571428</v>
+        <v>13.45974669312169</v>
       </c>
       <c r="E39">
-        <v>12.03885342261905</v>
+        <v>11.84950727513228</v>
       </c>
       <c r="F39">
-        <v>21.90329538690476</v>
+        <v>21.55939285714287</v>
       </c>
       <c r="G39">
-        <v>11.15032174776564</v>
+        <v>10.76782593250444</v>
       </c>
       <c r="H39">
-        <v>48.99193452380949</v>
+        <v>48.90767857142858</v>
       </c>
       <c r="I39">
-        <v>22.54017094017097</v>
+        <v>20.95153069806564</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1540,28 +1540,28 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>15.29884077380949</v>
+        <v>17.09604761904759</v>
       </c>
       <c r="C40">
-        <v>1.958020192307694</v>
+        <v>1.855968067226893</v>
       </c>
       <c r="D40">
-        <v>13.97191517857146</v>
+        <v>13.00694510582015</v>
       </c>
       <c r="E40">
-        <v>34.274238095238</v>
+        <v>31.58341865079355</v>
       </c>
       <c r="F40">
-        <v>43.61606770833334</v>
+        <v>42.94951388888888</v>
       </c>
       <c r="G40">
-        <v>14.38418111753371</v>
+        <v>13.98649999999999</v>
       </c>
       <c r="H40">
-        <v>84.54765624999997</v>
+        <v>91.55918650793645</v>
       </c>
       <c r="I40">
-        <v>26.98185873605948</v>
+        <v>29.05877824267785</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1569,28 +1569,28 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>17.32321726190478</v>
+        <v>19.01301917989419</v>
       </c>
       <c r="C41">
-        <v>2.988894308943095</v>
+        <v>2.792275104602516</v>
       </c>
       <c r="D41">
-        <v>16.10635788690477</v>
+        <v>15.01689947089948</v>
       </c>
       <c r="E41">
-        <v>25.47286979166669</v>
+        <v>27.8189093915344</v>
       </c>
       <c r="F41">
-        <v>45.62484375000003</v>
+        <v>48.59454828042335</v>
       </c>
       <c r="G41">
-        <v>17.23764123711339</v>
+        <v>17.27891988130563</v>
       </c>
       <c r="H41">
-        <v>58.39223214285706</v>
+        <v>70.25376322751312</v>
       </c>
       <c r="I41">
-        <v>16.3140363269425</v>
+        <v>26.50861767279093</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1598,28 +1598,28 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>17.1331123511905</v>
+        <v>20.19749206349209</v>
       </c>
       <c r="C42">
-        <v>3.653155097613886</v>
+        <v>4.28614070351759</v>
       </c>
       <c r="D42">
-        <v>19.9577581845238</v>
+        <v>19.63927465753425</v>
       </c>
       <c r="E42">
-        <v>32.28799851190472</v>
+        <v>36.82830687830685</v>
       </c>
       <c r="F42">
-        <v>53.45252752976194</v>
+        <v>54.78585780423283</v>
       </c>
       <c r="G42">
-        <v>22.95605504587155</v>
+        <v>23.69639399806388</v>
       </c>
       <c r="H42">
-        <v>102.0559747023811</v>
+        <v>112.212724867725</v>
       </c>
       <c r="I42">
-        <v>22.58063563115489</v>
+        <v>26.68007892659828</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1627,28 +1627,28 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>18.85414062500002</v>
+        <v>19.62552314814817</v>
       </c>
       <c r="C43">
-        <v>4.906473741794316</v>
+        <v>6.146785582255088</v>
       </c>
       <c r="D43">
-        <v>18.26681921331316</v>
+        <v>25.25435637583891</v>
       </c>
       <c r="E43">
-        <v>34.11799330357141</v>
+        <v>40.95738756613755</v>
       </c>
       <c r="F43">
-        <v>58.44974553571422</v>
+        <v>62.82951851851848</v>
       </c>
       <c r="G43">
-        <v>41.94808004158007</v>
+        <v>42.84417365269464</v>
       </c>
       <c r="H43">
-        <v>90.03922619047606</v>
+        <v>96.5359193121692</v>
       </c>
       <c r="I43">
-        <v>22.38691449814133</v>
+        <v>26.38018488745986</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1656,28 +1656,28 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>26.39734449404765</v>
+        <v>25.66541005291008</v>
       </c>
       <c r="C44">
-        <v>5.384380434782603</v>
+        <v>6.07775735294117</v>
       </c>
       <c r="D44">
-        <v>13.77982992565056</v>
+        <v>19.9122652733119</v>
       </c>
       <c r="E44">
-        <v>42.57393824404756</v>
+        <v>47.61254761904755</v>
       </c>
       <c r="F44">
-        <v>65.58478943452374</v>
+        <v>68.48221494708993</v>
       </c>
       <c r="G44">
-        <v>46.53277679697349</v>
+        <v>50.54092715920915</v>
       </c>
       <c r="H44">
-        <v>196.427611607143</v>
+        <v>189.3923280423283</v>
       </c>
       <c r="I44">
-        <v>40.45782775119619</v>
+        <v>39.81155668358718</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1685,28 +1685,28 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>24.94628348214287</v>
+        <v>24.18862734212355</v>
       </c>
       <c r="C45">
-        <v>5.831309443507594</v>
+        <v>6.164241621200315</v>
       </c>
       <c r="D45">
-        <v>20.07649652509649</v>
+        <v>20.36034482758618</v>
       </c>
       <c r="E45">
-        <v>43.35330729166656</v>
+        <v>41.80281339031328</v>
       </c>
       <c r="F45">
-        <v>92.568941220238</v>
+        <v>87.53804094378896</v>
       </c>
       <c r="G45">
-        <v>63.5691053698074</v>
+        <v>62.04829440628057</v>
       </c>
       <c r="H45">
-        <v>126.9600818452382</v>
+        <v>119.481783483692</v>
       </c>
       <c r="I45">
-        <v>30.94029810298099</v>
+        <v>28.8099252491694</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1714,28 +1714,28 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>27.01822023809522</v>
+        <v>26.43892195767194</v>
       </c>
       <c r="C46">
-        <v>6.655004175365346</v>
+        <v>6.576267980295566</v>
       </c>
       <c r="D46">
-        <v>22.85822003284076</v>
+        <v>22.76938023088026</v>
       </c>
       <c r="E46">
-        <v>47.56928794642862</v>
+        <v>42.70695833333338</v>
       </c>
       <c r="F46">
-        <v>84.35230431547643</v>
+        <v>76.74822420634943</v>
       </c>
       <c r="G46">
         <v>75.51658561967838</v>
       </c>
       <c r="H46">
-        <v>120.6320907738095</v>
+        <v>108.5622552910053</v>
       </c>
       <c r="I46">
-        <v>29.45944849959449</v>
+        <v>26.28927194860815</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1743,28 +1743,28 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>24.22775446428576</v>
+        <v>23.10210582010585</v>
       </c>
       <c r="C47">
-        <v>7.173578563995841</v>
+        <v>7.0229725177305</v>
       </c>
       <c r="D47">
-        <v>21.02328672985784</v>
+        <v>20.83090306834033</v>
       </c>
       <c r="E47">
-        <v>58.9504055059524</v>
+        <v>52.96374735449739</v>
       </c>
       <c r="F47">
-        <v>94.90857440476195</v>
+        <v>86.05269708994715</v>
       </c>
       <c r="G47">
         <v>90.60007589880146</v>
       </c>
       <c r="H47">
-        <v>134.5500076335879</v>
+        <v>120.431901217862</v>
       </c>
       <c r="I47">
-        <v>37.43856221198161</v>
+        <v>32.6687709497207</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1772,28 +1772,28 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>26.00445312500003</v>
+        <v>24.41901917989421</v>
       </c>
       <c r="C48">
-        <v>5.845127604166674</v>
+        <v>5.542611363636371</v>
       </c>
       <c r="D48">
-        <v>28.63865120132562</v>
+        <v>27.83480218181813</v>
       </c>
       <c r="E48">
-        <v>48.66932366071427</v>
+        <v>43.72148214285711</v>
       </c>
       <c r="F48">
-        <v>73.10094940476182</v>
+        <v>66.53717394179888</v>
       </c>
       <c r="G48">
         <v>110.2273069001032</v>
       </c>
       <c r="H48">
-        <v>106.6351029748284</v>
+        <v>95.49334009465855</v>
       </c>
       <c r="I48">
-        <v>34.46711802378763</v>
+        <v>30.1369785884218</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1801,28 +1801,28 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>24.68949851190478</v>
+        <v>23.21344841269844</v>
       </c>
       <c r="C49">
-        <v>6.211788759689923</v>
+        <v>5.585963333333334</v>
       </c>
       <c r="D49">
-        <v>20.64420282186948</v>
+        <v>20.84087557603685</v>
       </c>
       <c r="E49">
-        <v>54.79462202380954</v>
+        <v>49.133923941799</v>
       </c>
       <c r="F49">
-        <v>95.72711235119039</v>
+        <v>86.55589616402109</v>
       </c>
       <c r="G49">
-        <v>100.3258831030819</v>
+        <v>100.0071514830509</v>
       </c>
       <c r="H49">
-        <v>152.0036783320924</v>
+        <v>135.9181204500331</v>
       </c>
       <c r="I49">
-        <v>40.1567447916667</v>
+        <v>35.24637121212125</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1830,28 +1830,28 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>24.15414806547621</v>
+        <v>22.66934788359792</v>
       </c>
       <c r="C50">
-        <v>5.663728130360214</v>
+        <v>5.108230884557729</v>
       </c>
       <c r="D50">
-        <v>19.10263013698633</v>
+        <v>19.43023886639678</v>
       </c>
       <c r="E50">
-        <v>66.87306249999999</v>
+        <v>59.81433399470899</v>
       </c>
       <c r="F50">
-        <v>154.6788005952381</v>
+        <v>138.8606878306878</v>
       </c>
       <c r="G50">
-        <v>104.7166515151514</v>
+        <v>90.53443218954236</v>
       </c>
       <c r="H50">
-        <v>192.5542616679419</v>
+        <v>171.378806779661</v>
       </c>
       <c r="I50">
-        <v>35.19051235132662</v>
+        <v>30.69695479777953</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1859,28 +1859,28 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>23.48280877976195</v>
+        <v>21.9931375661376</v>
       </c>
       <c r="C51">
-        <v>5.469979683972909</v>
+        <v>4.981758183032729</v>
       </c>
       <c r="D51">
-        <v>24.71474479166662</v>
+        <v>24.357498015873</v>
       </c>
       <c r="E51">
-        <v>47.10871726190474</v>
+        <v>42.20976256613755</v>
       </c>
       <c r="F51">
-        <v>130.5186123511904</v>
+        <v>117.2996620370369</v>
       </c>
       <c r="G51">
-        <v>120.2305432389938</v>
+        <v>106.6528708333334</v>
       </c>
       <c r="H51">
-        <v>162.2824012158057</v>
+        <v>144.5836388140163</v>
       </c>
       <c r="I51">
-        <v>43.76580968280469</v>
+        <v>38.55095168374817</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1888,28 +1888,28 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>26.55422619047616</v>
+        <v>24.76079431216926</v>
       </c>
       <c r="C52">
-        <v>4.196375000000008</v>
+        <v>3.824733766233774</v>
       </c>
       <c r="D52">
-        <v>18.98235491071431</v>
+        <v>19.15651521164019</v>
       </c>
       <c r="E52">
-        <v>39.72758333333335</v>
+        <v>35.64118253968256</v>
       </c>
       <c r="F52">
-        <v>98.05047619047627</v>
+        <v>88.39108002645509</v>
       </c>
       <c r="G52">
-        <v>102.9899866999168</v>
+        <v>91.06461342086061</v>
       </c>
       <c r="H52">
-        <v>110.1258854166667</v>
+        <v>98.49761243386244</v>
       </c>
       <c r="I52">
-        <v>31.45610863095236</v>
+        <v>28.1003439153439</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1917,28 +1917,28 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>25.64778050595239</v>
+        <v>24.6043406084656</v>
       </c>
       <c r="C53">
-        <v>6.085201870615744</v>
+        <v>5.903855530474039</v>
       </c>
       <c r="D53">
-        <v>24.33714211309525</v>
+        <v>23.45866402116404</v>
       </c>
       <c r="E53">
-        <v>40.842599702381</v>
+        <v>36.90867923280427</v>
       </c>
       <c r="F53">
-        <v>107.9161577380952</v>
+        <v>97.14121230158727</v>
       </c>
       <c r="G53">
-        <v>92.77200822669114</v>
+        <v>81.72519584332541</v>
       </c>
       <c r="H53">
-        <v>114.0919490254872</v>
+        <v>101.9045406125166</v>
       </c>
       <c r="I53">
-        <v>30.93449631449635</v>
+        <v>27.33473722102235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>